<commit_message>
Sutvarkytos minimalios klaidos ir pirmas automatizuotas ifas su rizika
</commit_message>
<xml_diff>
--- a/Backend/IT_Klausimynas_UAB Bakalauras.xlsx
+++ b/Backend/IT_Klausimynas_UAB Bakalauras.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Įmonė:</t>
   </si>
@@ -46,30 +46,69 @@
     <t>Ar naudojama praėjimo kontrolės sistema?</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>dvsvdsv</t>
+  </si>
+  <si>
     <t>Kompiuterinio tinklo inventorizacija - Bendri klausimai</t>
   </si>
   <si>
     <t>Kokie tinklo įrangos gamintojai yra naudojami kompiuteriniame tinkle?</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>vdvdvdv</t>
+  </si>
+  <si>
     <t>Kaip užtikrinate, kad tinklo įrenginiai visada yra atnaujinti ir su naujaisiais pataisymais?</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>dsvsdvdsvs</t>
+  </si>
+  <si>
     <t>Ar naudojamas 802.1x protokolas?</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>vdsvsvsd</t>
+  </si>
+  <si>
+    <t>Ar prieiga prie tinklo įrenginių administravimo konsolės yra pasiekiama tik iš vidinio tinklo?</t>
+  </si>
+  <si>
+    <t>vdssdvds</t>
+  </si>
+  <si>
     <t>Ar pakeisti gamykliniai prisijungimo vardai ir slaptažodžiai?</t>
   </si>
   <si>
-    <t>Ar prieiga prie tinklo įrenginių administravimo konsolės yra pasiekiama tik iš vidinio tinklo?</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>vdsvsdvsd</t>
   </si>
   <si>
     <t>Kokiu būdu yra užtikrinamas slaptažodžių keitimas?</t>
   </si>
   <si>
+    <t>dsvsdvdsv</t>
+  </si>
+  <si>
     <t>Ar atliekamas vidinių sistemų skanavimas?</t>
   </si>
   <si>
+    <t>vsdvsdv</t>
+  </si>
+  <si>
     <t>Kompiuterinio tinklo inventorizacija - WiFi tinklas</t>
   </si>
   <si>
@@ -196,21 +235,21 @@
     <t>Ar naudojate IoT įrenginius?</t>
   </si>
   <si>
+    <t>Kokius ir kokiais tikslais?</t>
+  </si>
+  <si>
     <t>Ar naudojate GPS (vartotojo pozicijos nustatymo) sistemas bei įrangą?</t>
   </si>
   <si>
-    <t>Kokius ir kokiais tikslais?</t>
+    <t>Vartotojų naudojami įrenginiai - Kompiuterinės darbo vietos</t>
+  </si>
+  <si>
+    <t>Kompiuterizuotų darbo vietų skaičius</t>
   </si>
   <si>
     <t>Kokius ir kokiais tikslais, specializuota įranga ar mobilūs išmanieji tel.?</t>
   </si>
   <si>
-    <t>Vartotojų naudojami įrenginiai - Kompiuterinės darbo vietos</t>
-  </si>
-  <si>
-    <t>Kompiuterizuotų darbo vietų skaičius</t>
-  </si>
-  <si>
     <t>Naudojamos operacinės sistemos kompiuteriuose</t>
   </si>
   <si>
@@ -244,12 +283,12 @@
     <t>Kokios naudojamos programinės įrangos atnaujinimų priežiūros ir diegimo priemonės?</t>
   </si>
   <si>
+    <t>Ar sukonfigūruotas reguliarus skanavimas?</t>
+  </si>
+  <si>
     <t>Ar naudojama antivirusinė programinė įranga?</t>
   </si>
   <si>
-    <t>Ar sukonfigūruotas reguliarus skanavimas?</t>
-  </si>
-  <si>
     <t>Kokia antivirusinė naudojama?</t>
   </si>
   <si>
@@ -268,60 +307,60 @@
     <t>Kokios priemonės naudojamos apsisaugojimui nuo šifruojančių virusų?</t>
   </si>
   <si>
+    <t>Ar administratorius turi galimybę per nuotolį prisijungti prie vartotojo darbo aplinkos? Jei taip, ar vartotojas yra apie tai informuojamas, įspėjant apie galimą asmens duomenų atskleidimą?</t>
+  </si>
+  <si>
+    <t>Kaip yra pašalinami kompiuteriai, mobilieji įrenginiai, USB, kai jie nebenaudojami veikloje?</t>
+  </si>
+  <si>
     <t>Vartotojų naudojami įrenginiai - Vartotojų paskyrų valdymas</t>
   </si>
   <si>
     <t>Ar naudojama centralizuota vartotojų valdymo sistema (pvz. Active Directory)?</t>
   </si>
   <si>
+    <t>Kokia centralizuota vartotojų valdymo sistema naudojama?</t>
+  </si>
+  <si>
     <t>Ar visi vartotojai prijungti prie AD sistemos?</t>
   </si>
   <si>
-    <t>Kaip yra pašalinami kompiuteriai, mobilieji įrenginiai, USB, kai jie nebenaudojami veikloje?</t>
+    <t>Kokia tvarka yra naudojama valdant vartotojus (naujų paskyrų sukūrimas, išėjusių darbuotojų paskyrų pašalinimas, jei darbuotojas keičia poziciją - teisių pakeitimas, ir t.t.)?</t>
   </si>
   <si>
     <t>Ar jungiantis prie kompiuterių yra reikalaujama suvesti slaptažodžius?</t>
   </si>
   <si>
-    <t>Kokia centralizuota vartotojų valdymo sistema naudojama?</t>
+    <t>Ar naudojama multi-factor, bio autentifikacija?</t>
   </si>
   <si>
     <t>Ar yra slaptažodžių valdymo politika?</t>
   </si>
   <si>
-    <t>Ar administratorius turi galimybę per nuotolį prisijungti prie vartotojo darbo aplinkos? Jei taip, ar vartotojas yra apie tai informuojamas, įspėjant apie galimą asmens duomenų atskleidimą?</t>
-  </si>
-  <si>
     <t>Sudėtingumo faktoriaus patikrinimas?</t>
   </si>
   <si>
-    <t>Kokia tvarka yra naudojama valdant vartotojus (naujų paskyrų sukūrimas, išėjusių darbuotojų paskyrų pašalinimas, jei darbuotojas keičia poziciją - teisių pakeitimas, ir t.t.)?</t>
-  </si>
-  <si>
-    <t>Ar naudojama multi-factor, bio autentifikacija?</t>
-  </si>
-  <si>
     <t>Kartojamumo faktoriaus patikrinimas?</t>
   </si>
   <si>
+    <t>Periodinis keitimas?</t>
+  </si>
+  <si>
     <t>Lockout politika?</t>
   </si>
   <si>
-    <t>Periodinis keitimas?</t>
-  </si>
-  <si>
     <t>Ar  kompiuteriai automatiškai užsirakina po nustatyto periodo?</t>
   </si>
   <si>
     <t>Vartotojų naudojami įrenginiai - SIEM (Security Incident and Event Monitoring) sistemos</t>
   </si>
   <si>
+    <t>Ar yra naudojama centralizuota infrastruktūros ir saugumo įvykių (angl. 'logging') rinkimo, analizės ir pranešimų sistema (SIEM)?</t>
+  </si>
+  <si>
     <t>Kiek laiko saugoma informacija?</t>
   </si>
   <si>
-    <t>Ar yra naudojama centralizuota infrastruktūros ir saugumo įvykių (angl. 'logging') rinkimo, analizės ir pranešimų sistema (SIEM)?</t>
-  </si>
-  <si>
     <t>Ar yra kaupiama informacija iš visų įrenginių, kada koks vartotojas prisijungė, nepavykę prisijungimai?</t>
   </si>
   <si>
@@ -361,12 +400,12 @@
     <t>Ar šifruojami mobilieji įrenginiai?</t>
   </si>
   <si>
+    <t>Ar yra galimybė pašalinti duomenis nuotoliniu būdu iš pamesto įrenginio?</t>
+  </si>
+  <si>
     <t>Ar mobilieji įrenginiai yra atnaujinami automatiškai, kai gamintojas išleidžia atnaujinimą?</t>
   </si>
   <si>
-    <t>Ar yra galimybė pašalinti duomenis nuotoliniu būdu iš pamesto įrenginio?</t>
-  </si>
-  <si>
     <t>Ar mobiliuose įrenginiuose naudojama antivirusinė sistema? Jeigu taip, kokia?</t>
   </si>
   <si>
@@ -382,12 +421,12 @@
     <t>Tarnybinės stotys (vietiniame DC ir debesyje) - Valdymas ir priežiūra</t>
   </si>
   <si>
+    <t>Ar visi serveriai prijungti prie AD sistemos?</t>
+  </si>
+  <si>
     <t>Ar serveriai valdomi centralizuotai?</t>
   </si>
   <si>
-    <t>Ar visi serveriai prijungti prie AD sistemos?</t>
-  </si>
-  <si>
     <t>Kokiomis valdymo priemonėmis?</t>
   </si>
   <si>
@@ -397,6 +436,12 @@
     <t>Tarnybinės stotys (vietiniame DC ir debesyje) - Rezervinis kopijavimas</t>
   </si>
   <si>
+    <t>Kaip užtikrinamas veiklos tęstinumas ir rezervinis kopijavimas?</t>
+  </si>
+  <si>
+    <t>Ar naudojamas serverių ir serverių tarnybų darbingumo monitoringas? Jei taip, koks?</t>
+  </si>
+  <si>
     <t>Ar rezervinės kopijos šifruojamos?</t>
   </si>
   <si>
@@ -406,15 +451,9 @@
     <t>Kokiu periodiškumu bandoma atstatyti duomenis iš rezervinių kopijų?</t>
   </si>
   <si>
-    <t>Ar naudojamas serverių ir serverių tarnybų darbingumo monitoringas? Jei taip, koks?</t>
-  </si>
-  <si>
     <t>Ar yra offsite backup?</t>
   </si>
   <si>
-    <t>Kaip užtikrinamas veiklos tęstinumas ir rezervinis kopijavimas?</t>
-  </si>
-  <si>
     <t>Kokie vartotojai pasiekia rezervines kopijas?</t>
   </si>
   <si>
@@ -466,15 +505,21 @@
     <t>Kas prižiūri pateiktus tinklapius , taip pat kas administruoja ir hostina ?</t>
   </si>
   <si>
+    <t>Ar yra atliekami vertinimai svetainės atsparumams DDOS atakoms? Jeigu taip - kokiomis priemonėmis ir kokiu periodiškumu?</t>
+  </si>
+  <si>
+    <t>Tarnybinės stotys (vietiniame DC ir debesyje) - Duomenų bazės</t>
+  </si>
+  <si>
+    <t>Išvardinkite duomenų bazių sistemas, kurios yra naudojamos (su versijomis)</t>
+  </si>
+  <si>
     <t>Darbuotojai - Mokymai</t>
   </si>
   <si>
     <t>Ar vykdomi IT saugumo mokymai įmonės darbuotojams, jeigu taip - kokiu periodiškumu, ką apima mokymai (bendros saugumo politikos, phising atakos, kita)?</t>
   </si>
   <si>
-    <t>Ar yra atliekami vertinimai svetainės atsparumams DDOS atakoms? Jeigu taip - kokiomis priemonėmis ir kokiu periodiškumu?</t>
-  </si>
-  <si>
     <t>Ar yra atliktas socialinės inžinerijos (social engineering) testas?</t>
   </si>
   <si>
@@ -484,12 +529,6 @@
     <t>Ar partneriai / tiekėjai / klientai jungiasi prie jūsų vidinių informacinių sistemų? Jei taip, kokiu būdu ?</t>
   </si>
   <si>
-    <t>Tarnybinės stotys (vietiniame DC ir debesyje) - Duomenų bazės</t>
-  </si>
-  <si>
-    <t>Išvardinkite duomenų bazių sistemas, kurios yra naudojamos (su versijomis)</t>
-  </si>
-  <si>
     <t>Ar turi atskiras paskyras?</t>
   </si>
   <si>
@@ -514,10 +553,10 @@
     <t>Ar yra sprendimas dideliems failams?</t>
   </si>
   <si>
+    <t>Ar saugykla šifruota?</t>
+  </si>
+  <si>
     <t>Kaip dalinamasi failais su klientais / tiekėjais / partneriais?</t>
-  </si>
-  <si>
-    <t>Ar saugykla šifruota?</t>
   </si>
   <si>
     <t>Ar užtikrinama, kad tik paskirti asmenys atsidarys?</t>
@@ -951,1132 +990,1189 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B90" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B96" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B103" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B104" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B106" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B109" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B110" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B111" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B112" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="B113" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="B114" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="B115" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B116" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B117" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B118" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B119" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B121" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B122" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B124" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B125" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="B126" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B127" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B128" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B129" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B130" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B131" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B132" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B133" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B134" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B135" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B136" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B137" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B138" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B139" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B140" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="B141" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="B142" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B143" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dizainas ir toggle mygtukas
</commit_message>
<xml_diff>
--- a/Backend/IT_Klausimynas_UAB Bakalauras.xlsx
+++ b/Backend/IT_Klausimynas_UAB Bakalauras.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>Įmonė:</t>
   </si>
@@ -49,16 +49,16 @@
     <t>Ar naudojama praėjimo kontrolės sistema?</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>dscsac as</t>
-  </si>
-  <si>
-    <t>Netaikoma</t>
-  </si>
-  <si>
-    <t>Informacija</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>vdvs</t>
+  </si>
+  <si>
+    <t>Nėra</t>
+  </si>
+  <si>
+    <t>Aukšta</t>
   </si>
   <si>
     <t>Kompiuterinio tinklo inventorizacija - Bendri klausimai</t>
@@ -67,64 +67,58 @@
     <t>Kokie tinklo įrangos gamintojai yra naudojami kompiuteriniame tinkle?</t>
   </si>
   <si>
+    <t>vdssvsd</t>
+  </si>
+  <si>
+    <t>rekomendacijane</t>
+  </si>
+  <si>
+    <t>identifikuotarizika</t>
+  </si>
+  <si>
+    <t>Kaip užtikrinate, kad tinklo įrenginiai visada yra atnaujinti ir su naujaisiais pataisymais?</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>fewfwe</t>
+  </si>
+  <si>
+    <t>rekomendacijataip</t>
+  </si>
+  <si>
+    <t>Žema</t>
+  </si>
+  <si>
+    <t>Ar naudojamas 802.1x protokolas?</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>vds</t>
+  </si>
+  <si>
+    <t>Vidutinė</t>
+  </si>
+  <si>
+    <t>Ar prieiga prie tinklo įrenginių administravimo konsolės yra pasiekiama tik iš vidinio tinklo?</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>cascsacac</t>
-  </si>
-  <si>
-    <t>rekomendacijane</t>
-  </si>
-  <si>
-    <t>identifikuotarizika</t>
-  </si>
-  <si>
-    <t>Aukšta</t>
-  </si>
-  <si>
-    <t>Kaip užtikrinate, kad tinklo įrenginiai visada yra atnaujinti ir su naujaisiais pataisymais?</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>cascas</t>
-  </si>
-  <si>
-    <t>Ar naudojamas 802.1x protokolas?</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>cacas</t>
-  </si>
-  <si>
-    <t>Vidutinė</t>
-  </si>
-  <si>
-    <t>Ar prieiga prie tinklo įrenginių administravimo konsolės yra pasiekiama tik iš vidinio tinklo?</t>
+    <t>vsdvs</t>
+  </si>
+  <si>
+    <t>Ar pakeisti gamykliniai prisijungimo vardai ir slaptažodžiai?</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>cascsa</t>
-  </si>
-  <si>
-    <t>rekomendacijataip</t>
-  </si>
-  <si>
-    <t>Ar pakeisti gamykliniai prisijungimo vardai ir slaptažodžiai?</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>cascasa</t>
-  </si>
-  <si>
-    <t>Žema</t>
+    <t/>
   </si>
   <si>
     <t>Kokiu būdu yra užtikrinamas slaptažodžių keitimas?</t>
@@ -1048,19 +1042,19 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1068,22 +1062,22 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1100,10 +1094,10 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -1123,13 +1117,13 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1137,22 +1131,22 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,7 +1154,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,1071 +1162,1071 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
         <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
         <v>80</v>
-      </c>
-      <c r="B46" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
         <v>84</v>
-      </c>
-      <c r="B49" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" t="s">
         <v>108</v>
-      </c>
-      <c r="B72" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B80" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B83" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" t="s">
         <v>121</v>
-      </c>
-      <c r="B84" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B87" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B89" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B93" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B95" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B96" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B99" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>138</v>
+      </c>
+      <c r="B100" t="s">
         <v>140</v>
-      </c>
-      <c r="B100" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B101" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" t="s">
         <v>143</v>
-      </c>
-      <c r="B102" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B103" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B104" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B105" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B106" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>147</v>
+      </c>
+      <c r="B107" t="s">
         <v>149</v>
-      </c>
-      <c r="B107" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B111" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B112" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B113" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>155</v>
+      </c>
+      <c r="B114" t="s">
         <v>157</v>
-      </c>
-      <c r="B114" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B115" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>159</v>
+      </c>
+      <c r="B117" t="s">
         <v>161</v>
-      </c>
-      <c r="B117" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B118" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B122" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B123" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>167</v>
+      </c>
+      <c r="B124" t="s">
         <v>169</v>
-      </c>
-      <c r="B124" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B125" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B126" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B127" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>173</v>
+      </c>
+      <c r="B128" t="s">
         <v>175</v>
-      </c>
-      <c r="B128" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>176</v>
+      </c>
+      <c r="B130" t="s">
         <v>178</v>
-      </c>
-      <c r="B130" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B132" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B133" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B135" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B136" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B137" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B138" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B139" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B140" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B141" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B142" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B143" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>